<commit_message>
just another manic thursdayyyyyy
</commit_message>
<xml_diff>
--- a/documents/Book1.xlsx
+++ b/documents/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71dfea23b9759519/Python/console/card_stats/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="272" documentId="11_53EA479727D01CCACC2F65A6793802CEDDACD6DB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7303919F-672A-48CF-9EE2-29468F0C80ED}"/>
+  <xr:revisionPtr revIDLastSave="278" documentId="11_53EA479727D01CCACC2F65A6793802CEDDACD6DB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{938483F0-1455-4144-9C28-25792B47A946}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -170,7 +170,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -178,7 +178,6 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1149,25 +1148,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C2:AY78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M25" workbookViewId="0">
-      <selection activeCell="X48" sqref="X48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="46" max="51" width="9.140625" style="9"/>
+    <col min="46" max="51" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:51" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="AT2" s="8"/>
-      <c r="AU2" s="8"/>
-      <c r="AV2" s="8"/>
-      <c r="AW2" s="8"/>
-      <c r="AX2" s="8"/>
-      <c r="AY2" s="8"/>
+      <c r="AT2" s="7"/>
+      <c r="AU2" s="7"/>
+      <c r="AV2" s="7"/>
+      <c r="AW2" s="7"/>
+      <c r="AX2" s="7"/>
+      <c r="AY2" s="7"/>
     </row>
     <row r="4" spans="3:51" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
@@ -1184,10 +1183,10 @@
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1195,10 +1194,10 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1206,10 +1205,10 @@
       <c r="C7">
         <v>2</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>4.9186949530000003E-2</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1217,10 +1216,10 @@
       <c r="C8">
         <v>3</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>0.57265660750000003</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <f>SUM(D8:D13)</f>
         <v>0.95081304958629997</v>
       </c>
@@ -1229,10 +1228,10 @@
       <c r="C9">
         <v>4</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>0.30851659809999998</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <f>SUM(D9:D13)</f>
         <v>0.37815644208629995</v>
       </c>
@@ -1241,10 +1240,10 @@
       <c r="C10">
         <v>5</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>6.2518520820000006E-2</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <f>SUM(D10:D13)</f>
         <v>6.9639843986299993E-2</v>
       </c>
@@ -1253,10 +1252,10 @@
       <c r="C11">
         <v>6</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>6.7587590079999996E-3</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <f>SUM(D11:D13)</f>
         <v>7.1213231662999995E-3</v>
       </c>
@@ -1265,10 +1264,10 @@
       <c r="C12">
         <v>7</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="3">
         <v>3.5572415829999998E-4</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="3">
         <f>SUM(D12:D13)</f>
         <v>3.6256415829999996E-4</v>
       </c>
@@ -1277,10 +1276,10 @@
       <c r="C13">
         <v>8</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>6.8399999999999997E-6</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <f>SUM(D13)</f>
         <v>6.8399999999999997E-6</v>
       </c>
@@ -1297,12 +1296,12 @@
       <c r="C17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AT17" s="8"/>
-      <c r="AU17" s="8"/>
-      <c r="AV17" s="8"/>
-      <c r="AW17" s="8"/>
-      <c r="AX17" s="8"/>
-      <c r="AY17" s="8"/>
+      <c r="AT17" s="7"/>
+      <c r="AU17" s="7"/>
+      <c r="AV17" s="7"/>
+      <c r="AW17" s="7"/>
+      <c r="AX17" s="7"/>
+      <c r="AY17" s="7"/>
     </row>
     <row r="19" spans="3:51" x14ac:dyDescent="0.25">
       <c r="AT19"/>
@@ -2313,7 +2312,7 @@
         <f>V40*$V$36</f>
         <v>0.42593104288489525</v>
       </c>
-      <c r="W49" s="10">
+      <c r="W49" s="9">
         <f>W40*W$36</f>
         <v>0.18951983876477546</v>
       </c>
@@ -2350,7 +2349,7 @@
         <f t="shared" ref="U50:U53" si="8">U41*$U$36</f>
         <v>1.8051024586449221E-2</v>
       </c>
-      <c r="V50" s="10">
+      <c r="V50" s="9">
         <f t="shared" ref="V50:V53" si="9">V41*$V$36</f>
         <v>0.18138843519305517</v>
       </c>
@@ -2387,7 +2386,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="U51" s="10">
+      <c r="U51" s="9">
         <f t="shared" si="8"/>
         <v>4.4599462380738916E-3</v>
       </c>
@@ -2424,7 +2423,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T52" s="10">
+      <c r="T52" s="9">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -2461,7 +2460,7 @@
       <c r="R53">
         <v>5</v>
       </c>
-      <c r="S53" s="10">
+      <c r="S53" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2497,7 +2496,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AC53" s="7">
+      <c r="AC53" s="3">
         <f>SUM(S53,T52,U51,V50,W49,)</f>
         <v>0.37536822019590455</v>
       </c>
@@ -2509,12 +2508,12 @@
       <c r="C56" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="AT56" s="8"/>
-      <c r="AU56" s="8"/>
-      <c r="AV56" s="8"/>
-      <c r="AW56" s="8"/>
-      <c r="AX56" s="8"/>
-      <c r="AY56" s="8"/>
+      <c r="AT56" s="7"/>
+      <c r="AU56" s="7"/>
+      <c r="AV56" s="7"/>
+      <c r="AW56" s="7"/>
+      <c r="AX56" s="7"/>
+      <c r="AY56" s="7"/>
     </row>
     <row r="59" spans="3:51" x14ac:dyDescent="0.25">
       <c r="R59" t="s">
@@ -2885,6 +2884,66 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="S73:X78">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S23:AA28">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S39:AA44">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S48:AA53">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD23:AL28">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC53">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2896,43 +2955,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S23:AA28">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="0.5"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S39:AA44">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="0.5"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD23:AL28">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="0.5"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S48:AA53">
+  <conditionalFormatting sqref="D5:E13">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
fixed code but at what cost :/
</commit_message>
<xml_diff>
--- a/documents/Book1.xlsx
+++ b/documents/Book1.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71dfea23b9759519/Python/console/card_stats/documents/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_4D148DBE109723DD0E63FD6CD8A8D23FF70D2C11" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C227701-EDC5-4723-B342-043D8E0ED8F8}"/>
   <bookViews>
-    <workbookView xWindow="4155" yWindow="1080" windowWidth="33495" windowHeight="16935" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4155" yWindow="1080" windowWidth="29040" windowHeight="16440" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="31">
   <si>
     <t>0.0028  0.0015  0.0007  0.0003  0.002   0.0086  0.0194  -1      -1</t>
   </si>
@@ -118,13 +113,26 @@
   <si>
     <t>hm</t>
   </si>
+  <si>
+    <t>exacte</t>
+  </si>
+  <si>
+    <t>min unconditional</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>(3, 0, 2)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000%"/>
+    <numFmt numFmtId="165" formatCode="0.0000000000000000%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -185,7 +193,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -195,6 +203,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -218,9 +228,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -258,7 +268,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -330,7 +340,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -503,7 +513,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="I7:Y30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1159,15 +1169,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="C2:AY103"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:AY113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="R30" sqref="R30"/>
+    <sheetView topLeftCell="E63" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I97" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="46" max="51" width="9.140625" style="7"/>
   </cols>
   <sheetData>
@@ -1914,15 +1925,9 @@
     <row r="32" spans="3:51" x14ac:dyDescent="0.25">
       <c r="AU32"/>
     </row>
-    <row r="33" spans="3:47" x14ac:dyDescent="0.25">
-      <c r="AT33"/>
-      <c r="AU33"/>
-    </row>
-    <row r="34" spans="3:47" x14ac:dyDescent="0.25">
-      <c r="AT34"/>
-      <c r="AU34"/>
-    </row>
-    <row r="36" spans="3:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="3:47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="3:47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="S36">
         <v>0</v>
       </c>
@@ -1950,13 +1955,17 @@
       <c r="AA36" s="3">
         <v>6.8399999999999997E-6</v>
       </c>
-    </row>
-    <row r="37" spans="3:47" x14ac:dyDescent="0.25">
+      <c r="AT36" s="7"/>
+      <c r="AU36" s="7"/>
+    </row>
+    <row r="37" spans="3:47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="S37" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="38" spans="3:47" x14ac:dyDescent="0.25">
+      <c r="AT37" s="7"/>
+      <c r="AU37" s="7"/>
+    </row>
+    <row r="38" spans="3:47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="R38" t="s">
         <v>4</v>
       </c>
@@ -1987,8 +1996,10 @@
       <c r="AA38">
         <v>8</v>
       </c>
-    </row>
-    <row r="39" spans="3:47" x14ac:dyDescent="0.25">
+      <c r="AT38" s="7"/>
+      <c r="AU38" s="7"/>
+    </row>
+    <row r="39" spans="3:47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q39" t="s">
         <v>5</v>
       </c>
@@ -2031,8 +2042,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="3:47" x14ac:dyDescent="0.25">
+      <c r="AT39" s="7"/>
+      <c r="AU39" s="7"/>
+    </row>
+    <row r="40" spans="3:47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="R40">
         <v>1</v>
       </c>
@@ -2072,8 +2085,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="3:47" x14ac:dyDescent="0.25">
+      <c r="AT40" s="7"/>
+      <c r="AU40" s="7"/>
+    </row>
+    <row r="41" spans="3:47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="R41">
         <v>2</v>
       </c>
@@ -2113,8 +2128,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="3:47" x14ac:dyDescent="0.25">
+      <c r="AT41" s="7"/>
+      <c r="AU41" s="7"/>
+    </row>
+    <row r="42" spans="3:47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="R42">
         <v>3</v>
       </c>
@@ -2154,8 +2171,10 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="3:47" x14ac:dyDescent="0.25">
+      <c r="AT42" s="7"/>
+      <c r="AU42" s="7"/>
+    </row>
+    <row r="43" spans="3:47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="R43">
         <v>4</v>
       </c>
@@ -2195,8 +2214,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="3:47" x14ac:dyDescent="0.25">
+      <c r="AT43" s="7"/>
+      <c r="AU43" s="7"/>
+    </row>
+    <row r="44" spans="3:47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="R44">
         <v>5</v>
       </c>
@@ -2236,13 +2257,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="3:47" x14ac:dyDescent="0.25">
+      <c r="AT44" s="7"/>
+      <c r="AU44" s="7"/>
+    </row>
+    <row r="46" spans="3:47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="S46" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="47" spans="3:47" x14ac:dyDescent="0.25">
+      <c r="AT46" s="7"/>
+      <c r="AU46" s="7"/>
+    </row>
+    <row r="47" spans="3:47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C47">
         <v>5</v>
       </c>
@@ -2276,8 +2301,10 @@
       <c r="AA47">
         <v>8</v>
       </c>
-    </row>
-    <row r="48" spans="3:47" x14ac:dyDescent="0.25">
+      <c r="AT47" s="7"/>
+      <c r="AU47" s="7"/>
+    </row>
+    <row r="48" spans="3:47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q48" t="s">
         <v>5</v>
       </c>
@@ -2320,8 +2347,10 @@
         <f t="shared" ref="AA48:AA53" si="14">AA39*$AA$36</f>
         <v>6.8399999999999997E-6</v>
       </c>
-    </row>
-    <row r="49" spans="14:29" x14ac:dyDescent="0.25">
+      <c r="AT48" s="7"/>
+      <c r="AU48" s="7"/>
+    </row>
+    <row r="49" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="N49" s="3"/>
       <c r="R49">
         <v>1</v>
@@ -2363,7 +2392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="14:29" x14ac:dyDescent="0.25">
+    <row r="50" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="R50">
         <v>2</v>
       </c>
@@ -2404,7 +2433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="14:29" x14ac:dyDescent="0.25">
+    <row r="51" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="R51">
         <v>3</v>
       </c>
@@ -2445,7 +2474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="14:29" x14ac:dyDescent="0.25">
+    <row r="52" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="R52">
         <v>4</v>
       </c>
@@ -2486,7 +2515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="14:29" x14ac:dyDescent="0.25">
+    <row r="53" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="R53">
         <v>5</v>
       </c>
@@ -2531,7 +2560,7 @@
         <v>0.37536822019590455</v>
       </c>
     </row>
-    <row r="54" spans="14:29" x14ac:dyDescent="0.25">
+    <row r="54" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="S54" s="8"/>
       <c r="T54" s="2"/>
       <c r="U54" s="2"/>
@@ -2543,7 +2572,7 @@
       <c r="AA54" s="2"/>
       <c r="AC54" s="2"/>
     </row>
-    <row r="55" spans="14:29" x14ac:dyDescent="0.25">
+    <row r="55" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="S55" s="2" t="s">
         <v>25</v>
       </c>
@@ -2557,7 +2586,7 @@
       <c r="AA55" s="2"/>
       <c r="AC55" s="2"/>
     </row>
-    <row r="56" spans="14:29" x14ac:dyDescent="0.25">
+    <row r="56" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="R56" t="s">
         <v>4</v>
       </c>
@@ -2590,7 +2619,7 @@
       </c>
       <c r="AC56" s="2"/>
     </row>
-    <row r="57" spans="14:29" x14ac:dyDescent="0.25">
+    <row r="57" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q57" t="s">
         <v>5</v>
       </c>
@@ -2635,7 +2664,7 @@
       </c>
       <c r="AC57" s="2"/>
     </row>
-    <row r="58" spans="14:29" x14ac:dyDescent="0.25">
+    <row r="58" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="R58">
         <v>1</v>
       </c>
@@ -2677,7 +2706,7 @@
       </c>
       <c r="AC58" s="2"/>
     </row>
-    <row r="59" spans="14:29" x14ac:dyDescent="0.25">
+    <row r="59" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="R59">
         <v>2</v>
       </c>
@@ -2719,7 +2748,7 @@
       </c>
       <c r="AC59" s="2"/>
     </row>
-    <row r="60" spans="14:29" x14ac:dyDescent="0.25">
+    <row r="60" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="R60">
         <v>3</v>
       </c>
@@ -2761,7 +2790,7 @@
       </c>
       <c r="AC60" s="2"/>
     </row>
-    <row r="61" spans="14:29" x14ac:dyDescent="0.25">
+    <row r="61" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="R61">
         <v>4</v>
       </c>
@@ -2803,7 +2832,7 @@
       </c>
       <c r="AC61" s="2"/>
     </row>
-    <row r="62" spans="14:29" x14ac:dyDescent="0.25">
+    <row r="62" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="R62">
         <v>5</v>
       </c>
@@ -2845,10 +2874,10 @@
       </c>
       <c r="AC62" s="2"/>
     </row>
-    <row r="63" spans="14:29" x14ac:dyDescent="0.25">
+    <row r="63" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="AC63" s="2"/>
     </row>
-    <row r="64" spans="14:29" x14ac:dyDescent="0.25">
+    <row r="64" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="AC64" s="2"/>
     </row>
     <row r="65" spans="3:51" x14ac:dyDescent="0.25">
@@ -2913,6 +2942,9 @@
       <c r="X71" s="2">
         <v>0.33318743845059601</v>
       </c>
+      <c r="Z71" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="72" spans="3:51" x14ac:dyDescent="0.25">
       <c r="R72">
@@ -3032,480 +3064,553 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="17:24" x14ac:dyDescent="0.25">
-      <c r="S82" s="2">
+    <row r="84" spans="9:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R84" t="s">
+        <v>21</v>
+      </c>
+      <c r="S84" t="s">
+        <v>15</v>
+      </c>
+      <c r="T84" t="s">
+        <v>16</v>
+      </c>
+      <c r="U84" t="s">
+        <v>17</v>
+      </c>
+      <c r="V84" t="s">
+        <v>18</v>
+      </c>
+      <c r="W84" t="s">
+        <v>19</v>
+      </c>
+      <c r="X84" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="85" spans="9:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q85" t="s">
+        <v>14</v>
+      </c>
+      <c r="R85">
+        <v>0</v>
+      </c>
+      <c r="S85" s="2">
+        <f>S72</f>
+        <v>0.39118065433854898</v>
+      </c>
+    </row>
+    <row r="86" spans="9:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="9:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="9:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="9:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R89">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="9:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R90">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="9:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S92" s="2">
         <f>U57</f>
         <v>1.0749307420987755E-2</v>
       </c>
-      <c r="T82" s="2">
+      <c r="T92" s="2">
         <f>V57</f>
         <v>0.14672556461510369</v>
       </c>
-      <c r="U82" s="2">
+      <c r="U92" s="2">
         <f>W57</f>
         <v>0.1189967593352238</v>
       </c>
-      <c r="V82" s="2">
+      <c r="V92" s="2">
         <f>U58</f>
         <v>2.0386617522562964E-2</v>
       </c>
-      <c r="W82" s="2">
+      <c r="W92" s="2">
         <f>V58</f>
         <v>0.24454260769184005</v>
       </c>
-      <c r="X82" s="2">
+      <c r="X92" s="2">
         <f>U59</f>
         <v>1.3591078348375328E-2</v>
       </c>
     </row>
-    <row r="83" spans="17:24" x14ac:dyDescent="0.25">
-      <c r="Q83" t="s">
+    <row r="93" spans="9:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I93" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q93" t="s">
         <v>14</v>
       </c>
-      <c r="R83" t="s">
+      <c r="R93" t="s">
         <v>21</v>
       </c>
-      <c r="S83" t="s">
+      <c r="S93" t="s">
         <v>15</v>
       </c>
-      <c r="T83" t="s">
+      <c r="T93" t="s">
         <v>16</v>
       </c>
-      <c r="U83" t="s">
+      <c r="U93" t="s">
         <v>17</v>
       </c>
-      <c r="V83" t="s">
+      <c r="V93" t="s">
         <v>18</v>
       </c>
-      <c r="W83" t="s">
+      <c r="W93" t="s">
         <v>19</v>
       </c>
-      <c r="X83" t="s">
+      <c r="X93" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="84" spans="17:24" x14ac:dyDescent="0.25">
-      <c r="R84">
-        <v>0</v>
-      </c>
-      <c r="S84" s="2">
+    <row r="94" spans="9:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I94" s="9">
+        <f>T73*T92</f>
+        <v>4.1903241453706164E-2</v>
+      </c>
+      <c r="R94">
+        <v>0</v>
+      </c>
+      <c r="S94" s="2">
         <f>SUM(S71:S76)</f>
         <v>0.999999999999998</v>
       </c>
-      <c r="T84" s="2">
+      <c r="T94" s="2">
         <f>SUM(T71:T76)</f>
         <v>0.99999999999999845</v>
       </c>
-      <c r="U84" s="2">
-        <f t="shared" ref="U84:X84" si="24">SUM(U71:U76)</f>
+      <c r="U94" s="2">
+        <f t="shared" ref="U94:X94" si="24">SUM(U71:U76)</f>
         <v>0.99999999999999822</v>
       </c>
-      <c r="V84" s="2">
+      <c r="V94" s="2">
         <f t="shared" si="24"/>
         <v>0.99999999999999845</v>
       </c>
-      <c r="W84" s="2">
+      <c r="W94" s="2">
         <f t="shared" si="24"/>
         <v>0.99999999999999878</v>
       </c>
-      <c r="X84" s="2">
+      <c r="X94" s="2">
         <f t="shared" si="24"/>
         <v>0.99999999999999878</v>
       </c>
-    </row>
-    <row r="85" spans="17:24" x14ac:dyDescent="0.25">
-      <c r="R85">
+      <c r="Z94" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="95" spans="9:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R95">
         <v>1</v>
       </c>
-      <c r="S85" s="2">
-        <f t="shared" ref="S85:T85" si="25">SUM(S72:S77)</f>
+      <c r="S95" s="10">
+        <f t="shared" ref="S95:T95" si="25">SUM(S72:S77)</f>
         <v>0.829302987197723</v>
       </c>
-      <c r="T85" s="2">
+      <c r="T95" s="2">
         <f t="shared" si="25"/>
         <v>0.79374110953058252</v>
       </c>
-      <c r="U85" s="2">
-        <f t="shared" ref="U85:X85" si="26">SUM(U72:U77)</f>
+      <c r="U95" s="2">
+        <f t="shared" ref="U95:X95" si="26">SUM(U72:U77)</f>
         <v>0.65570631360104925</v>
       </c>
-      <c r="V85" s="2">
+      <c r="V95" s="2">
         <f t="shared" si="26"/>
         <v>0.79374110953058252</v>
       </c>
-      <c r="W85" s="2">
+      <c r="W95" s="2">
         <f t="shared" si="26"/>
         <v>0.66681256154940272</v>
       </c>
-      <c r="X85" s="2">
+      <c r="X95" s="2">
         <f t="shared" si="26"/>
         <v>0.66681256154940272</v>
       </c>
     </row>
-    <row r="86" spans="17:24" x14ac:dyDescent="0.25">
-      <c r="R86">
+    <row r="96" spans="9:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R96">
         <v>2</v>
       </c>
-      <c r="S86" s="2">
-        <f t="shared" ref="S86:T86" si="27">SUM(S73:S78)</f>
+      <c r="S96" s="2">
+        <f t="shared" ref="S96:T96" si="27">SUM(S73:S78)</f>
         <v>0.43812233285917407</v>
       </c>
-      <c r="T86" s="2">
+      <c r="T96" s="2">
         <f t="shared" si="27"/>
         <v>0.38122332859174957</v>
       </c>
-      <c r="U86" s="2">
-        <f t="shared" ref="U86:X86" si="28">SUM(U73:U78)</f>
+      <c r="U96" s="2">
+        <f t="shared" ref="U96:X96" si="28">SUM(U73:U78)</f>
         <v>0.21304300251668626</v>
       </c>
-      <c r="V86" s="2">
+      <c r="V96" s="2">
         <f t="shared" si="28"/>
         <v>0.38122332859174957</v>
       </c>
-      <c r="W86" s="2">
+      <c r="W96" s="2">
         <f t="shared" si="28"/>
         <v>0.22256264361527475</v>
       </c>
-      <c r="X86" s="2">
+      <c r="X96" s="2">
         <f t="shared" si="28"/>
         <v>0.22256264361527475</v>
       </c>
     </row>
-    <row r="87" spans="17:24" x14ac:dyDescent="0.25">
-      <c r="R87">
+    <row r="97" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R97">
         <v>3</v>
       </c>
-      <c r="S87" s="2">
-        <f t="shared" ref="S87:T87" si="29">SUM(S74:S79)</f>
+      <c r="S97" s="2">
+        <f t="shared" ref="S97:T97" si="29">SUM(S74:S79)</f>
         <v>0.12517780938833503</v>
       </c>
-      <c r="T87" s="2">
+      <c r="T97" s="2">
         <f t="shared" si="29"/>
         <v>9.563409563409557E-2</v>
       </c>
-      <c r="U87" s="2">
-        <f t="shared" ref="U87:X87" si="30">SUM(U74:U79)</f>
+      <c r="U97" s="2">
+        <f t="shared" ref="U97:X97" si="30">SUM(U74:U79)</f>
         <v>2.987197724039823E-2</v>
       </c>
-      <c r="V87" s="2">
+      <c r="V97" s="2">
         <f t="shared" si="30"/>
         <v>9.563409563409557E-2</v>
       </c>
-      <c r="W87" s="2">
+      <c r="W97" s="2">
         <f t="shared" si="30"/>
         <v>3.2169821643505771E-2</v>
       </c>
-      <c r="X87" s="2">
+      <c r="X97" s="2">
         <f t="shared" si="30"/>
         <v>3.2169821643505771E-2</v>
       </c>
     </row>
-    <row r="88" spans="17:24" x14ac:dyDescent="0.25">
-      <c r="R88">
+    <row r="98" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R98">
         <v>4</v>
       </c>
-      <c r="S88" s="2">
-        <f t="shared" ref="S88:T88" si="31">SUM(S75:S80)</f>
+      <c r="S98" s="2">
+        <f t="shared" ref="S98:T98" si="31">SUM(S75:S80)</f>
         <v>1.6850858956122036E-2</v>
       </c>
-      <c r="T88" s="2">
+      <c r="T98" s="2">
         <f t="shared" si="31"/>
         <v>1.1015063646642564E-2</v>
       </c>
-      <c r="U88" s="2">
-        <f t="shared" ref="U88:X88" si="32">SUM(U75:U80)</f>
+      <c r="U98" s="2">
+        <f t="shared" ref="U98:X98" si="32">SUM(U75:U80)</f>
         <v>1.37870664186453E-3</v>
       </c>
-      <c r="V88" s="2">
+      <c r="V98" s="2">
         <f t="shared" si="32"/>
         <v>1.1015063646642564E-2</v>
       </c>
-      <c r="W88" s="2">
+      <c r="W98" s="2">
         <f t="shared" si="32"/>
         <v>1.5318962687383699E-3</v>
       </c>
-      <c r="X88" s="2">
+      <c r="X98" s="2">
         <f t="shared" si="32"/>
         <v>1.5318962687383699E-3</v>
       </c>
     </row>
-    <row r="89" spans="17:24" x14ac:dyDescent="0.25">
-      <c r="R89">
+    <row r="99" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R99">
         <v>5</v>
       </c>
-      <c r="S89" s="2">
-        <f t="shared" ref="S89:T89" si="33">SUM(S76:S81)</f>
-        <v>8.0242185505343397E-4</v>
-      </c>
-      <c r="T89" s="2">
+      <c r="S99" s="2">
+        <f t="shared" ref="S99:T99" si="33">SUM(S76:S91)</f>
+        <v>0.3919830761936024</v>
+      </c>
+      <c r="T99" s="2">
         <f t="shared" si="33"/>
         <v>4.37684648210964E-4</v>
       </c>
-      <c r="U89" s="2">
-        <f t="shared" ref="U89:X89" si="34">SUM(U76:U81)</f>
-        <v>0</v>
-      </c>
-      <c r="V89" s="2">
+      <c r="U99" s="2">
+        <f t="shared" ref="U99:X99" si="34">SUM(U76:U91)</f>
+        <v>0</v>
+      </c>
+      <c r="V99" s="2">
         <f t="shared" si="34"/>
         <v>4.37684648210964E-4</v>
       </c>
-      <c r="W89" s="2">
-        <f>SUM(W76:W81)</f>
-        <v>0</v>
-      </c>
-      <c r="X89" s="2">
+      <c r="W99" s="2">
+        <f>SUM(W76:W91)</f>
+        <v>0</v>
+      </c>
+      <c r="X99" s="2">
         <f t="shared" si="34"/>
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="17:24" x14ac:dyDescent="0.25">
-      <c r="Q92" t="s">
+    <row r="102" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q102" t="s">
         <v>14</v>
       </c>
-      <c r="R92" t="s">
+      <c r="R102" t="s">
         <v>21</v>
       </c>
-      <c r="S92" t="s">
+      <c r="S102" t="s">
         <v>15</v>
       </c>
-      <c r="T92" t="s">
+      <c r="T102" t="s">
         <v>16</v>
       </c>
-      <c r="U92" t="s">
+      <c r="U102" t="s">
         <v>17</v>
       </c>
-      <c r="V92" t="s">
+      <c r="V102" t="s">
         <v>18</v>
       </c>
-      <c r="W92" t="s">
+      <c r="W102" t="s">
         <v>19</v>
       </c>
-      <c r="X92" t="s">
+      <c r="X102" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="17:24" x14ac:dyDescent="0.25">
-      <c r="R93">
-        <v>0</v>
-      </c>
-      <c r="S93" s="2">
-        <f>$S$82*S84</f>
+    <row r="103" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R103">
+        <v>0</v>
+      </c>
+      <c r="S103" s="2">
+        <f>$S$92*S94</f>
         <v>1.0749307420987734E-2</v>
       </c>
-      <c r="T93" s="2">
-        <f>$T$82*T84</f>
+      <c r="T103" s="2">
+        <f>$T$92*T94</f>
         <v>0.14672556461510347</v>
       </c>
-      <c r="U93" s="2">
-        <f>$U$82*U84</f>
+      <c r="U103" s="2">
+        <f>$U$92*U94</f>
         <v>0.11899675933522359</v>
       </c>
-      <c r="V93" s="2">
-        <f>$V$82*V84</f>
+      <c r="V103" s="2">
+        <f>$V$92*V94</f>
         <v>2.0386617522562933E-2</v>
       </c>
-      <c r="W93" s="2">
-        <f>$W$82*W84</f>
+      <c r="W103" s="2">
+        <f>$W$92*W94</f>
         <v>0.24454260769183975</v>
       </c>
-      <c r="X93" s="2">
-        <f>$X$82*X84</f>
+      <c r="X103" s="2">
+        <f>$X$92*X94</f>
         <v>1.3591078348375311E-2</v>
       </c>
-    </row>
-    <row r="94" spans="17:24" x14ac:dyDescent="0.25">
-      <c r="R94">
+      <c r="Z103" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="104" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R104">
         <v>1</v>
       </c>
-      <c r="S94" s="2">
-        <f t="shared" ref="S94:S98" si="35">$S$82*S85</f>
+      <c r="S104" s="2">
+        <f t="shared" ref="S104:S108" si="35">$S$92*S95</f>
         <v>8.9144327545317963E-3</v>
       </c>
-      <c r="T94" s="2">
-        <f t="shared" ref="T94:T98" si="36">$T$82*T85</f>
+      <c r="T104" s="2">
+        <f t="shared" ref="T104:T108" si="36">$T$92*T95</f>
         <v>0.11646211245409359</v>
       </c>
-      <c r="U94" s="2">
-        <f t="shared" ref="U94:U98" si="37">$U$82*U85</f>
+      <c r="U104" s="8">
+        <f t="shared" ref="U104:U108" si="37">$U$92*U95</f>
         <v>7.8026926394170845E-2</v>
       </c>
-      <c r="V94" s="2">
-        <f t="shared" ref="V94:V98" si="38">$V$82*V85</f>
+      <c r="V104" s="2">
+        <f t="shared" ref="V104:V108" si="38">$V$92*V95</f>
         <v>1.6181696411934742E-2</v>
       </c>
-      <c r="W94" s="2">
-        <f t="shared" ref="W94:W98" si="39">$W$82*W85</f>
+      <c r="W104" s="8">
+        <f t="shared" ref="W104:W108" si="39">$W$92*W95</f>
         <v>0.16306408264296654</v>
       </c>
-      <c r="X94" s="2">
-        <f t="shared" ref="X94:X98" si="40">$X$82*X85</f>
+      <c r="X104" s="8">
+        <f t="shared" ref="X104:X108" si="40">$X$92*X95</f>
         <v>9.0627017676987772E-3</v>
       </c>
     </row>
-    <row r="95" spans="17:24" x14ac:dyDescent="0.25">
-      <c r="R95">
+    <row r="105" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R105">
         <v>2</v>
       </c>
-      <c r="S95" s="2">
+      <c r="S105" s="2">
         <f t="shared" si="35"/>
         <v>4.7095116439035871E-3</v>
       </c>
-      <c r="T95" s="2">
+      <c r="T105" s="8">
         <f t="shared" si="36"/>
         <v>5.5935208132073658E-2</v>
       </c>
-      <c r="U95" s="2">
+      <c r="U105" s="2">
         <f t="shared" si="37"/>
         <v>2.5351426898531593E-2</v>
       </c>
-      <c r="V95" s="2">
+      <c r="V105" s="8">
         <f t="shared" si="38"/>
         <v>7.7718541906783402E-3</v>
       </c>
-      <c r="W95" s="2">
+      <c r="W105" s="2">
         <f t="shared" si="39"/>
         <v>5.4426049244468942E-2</v>
       </c>
-      <c r="X95" s="2">
+      <c r="X105" s="2">
         <f t="shared" si="40"/>
         <v>3.0248663267967353E-3</v>
       </c>
     </row>
-    <row r="96" spans="17:24" x14ac:dyDescent="0.25">
-      <c r="R96">
+    <row r="106" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R106">
         <v>3</v>
       </c>
-      <c r="S96" s="2">
+      <c r="S106" s="8">
         <f t="shared" si="35"/>
         <v>1.3455747554010204E-3</v>
       </c>
-      <c r="T96" s="2">
+      <c r="T106" s="2">
         <f t="shared" si="36"/>
         <v>1.4031966678367496E-2</v>
       </c>
-      <c r="U96" s="2">
+      <c r="U106" s="2">
         <f t="shared" si="37"/>
         <v>3.5546684865429509E-3</v>
       </c>
-      <c r="V96" s="2">
+      <c r="V106" s="2">
         <f t="shared" si="38"/>
         <v>1.9496557298085151E-3</v>
       </c>
-      <c r="W96" s="2">
+      <c r="W106" s="2">
         <f t="shared" si="39"/>
         <v>7.8668920736842968E-3</v>
       </c>
-      <c r="X96" s="2">
+      <c r="X106" s="2">
         <f t="shared" si="40"/>
         <v>4.3722256641014727E-4</v>
       </c>
     </row>
-    <row r="97" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R97">
+    <row r="107" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R107">
         <v>4</v>
       </c>
-      <c r="S97" s="2">
+      <c r="S107" s="2">
         <f t="shared" si="35"/>
         <v>1.8113506322706057E-4</v>
       </c>
-      <c r="T97" s="2">
+      <c r="T107" s="2">
         <f t="shared" si="36"/>
         <v>1.6161914328249333E-3</v>
       </c>
-      <c r="U97" s="2">
+      <c r="U107" s="2">
         <f t="shared" si="37"/>
         <v>1.6406162245582808E-4</v>
       </c>
-      <c r="V97" s="2">
+      <c r="V107" s="2">
         <f t="shared" si="38"/>
         <v>2.245598895507896E-4</v>
       </c>
-      <c r="W97" s="2">
+      <c r="W107" s="2">
         <f t="shared" si="39"/>
         <v>3.7461390827068077E-4</v>
       </c>
-      <c r="X97" s="2">
+      <c r="X107" s="2">
         <f t="shared" si="40"/>
         <v>2.0820122210007011E-5</v>
       </c>
     </row>
-    <row r="98" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="R98">
+    <row r="108" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R108">
         <v>5</v>
       </c>
-      <c r="S98" s="2">
+      <c r="S108" s="2">
         <f t="shared" si="35"/>
-        <v>8.6254792012886384E-6</v>
-      </c>
-      <c r="T98" s="2">
+        <v>4.2135465898294989E-3</v>
+      </c>
+      <c r="T108" s="2">
         <f t="shared" si="36"/>
         <v>6.4219527132116727E-5</v>
       </c>
-      <c r="U98" s="2">
+      <c r="U108" s="2">
         <f t="shared" si="37"/>
         <v>0</v>
       </c>
-      <c r="V98" s="2">
+      <c r="V108" s="2">
         <f t="shared" si="38"/>
         <v>8.9229095185744448E-6</v>
       </c>
-      <c r="W98" s="2">
+      <c r="W108" s="2">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="X98" s="2">
+      <c r="X108" s="2">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="Z98" s="2">
-        <f>SUM(S96,T95,U94,V95,W94,X94)</f>
+      <c r="Z108" s="2">
+        <f>SUM(S106,T105,U104,V105,W104,X104)</f>
         <v>0.31520634788298924</v>
       </c>
-      <c r="AA98" s="2"/>
-      <c r="AB98" s="2"/>
-      <c r="AC98" s="2"/>
-      <c r="AD98" s="2"/>
-      <c r="AE98" s="2"/>
-    </row>
-    <row r="99" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="Z99" s="2"/>
-      <c r="AA99" s="2"/>
-      <c r="AB99" s="2"/>
-      <c r="AC99" s="2"/>
-      <c r="AD99" s="2"/>
-      <c r="AE99" s="2"/>
-    </row>
-    <row r="100" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="Z100" s="2"/>
-      <c r="AA100" s="2"/>
-      <c r="AB100" s="2"/>
-      <c r="AC100" s="2"/>
-      <c r="AD100" s="2"/>
-      <c r="AE100" s="2"/>
-    </row>
-    <row r="101" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="Z101" s="2"/>
-      <c r="AA101" s="2"/>
-      <c r="AB101" s="2"/>
-      <c r="AC101" s="2"/>
-      <c r="AD101" s="2"/>
-      <c r="AE101" s="2"/>
-    </row>
-    <row r="102" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="Z102" s="2"/>
-      <c r="AA102" s="2"/>
-      <c r="AB102" s="2"/>
-      <c r="AC102" s="2"/>
-      <c r="AD102" s="2"/>
-      <c r="AE102" s="2"/>
-    </row>
-    <row r="103" spans="18:31" x14ac:dyDescent="0.25">
-      <c r="Z103" s="2"/>
-      <c r="AA103" s="2"/>
-      <c r="AB103" s="2"/>
-      <c r="AC103" s="2"/>
-      <c r="AD103" s="2"/>
-      <c r="AE103" s="2"/>
+      <c r="AA108" s="2"/>
+      <c r="AB108" s="2"/>
+      <c r="AC108" s="2"/>
+      <c r="AD108" s="2"/>
+      <c r="AE108" s="2"/>
+    </row>
+    <row r="109" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z109" s="2"/>
+      <c r="AA109" s="2"/>
+      <c r="AB109" s="2"/>
+      <c r="AC109" s="2"/>
+      <c r="AD109" s="2"/>
+      <c r="AE109" s="2"/>
+    </row>
+    <row r="110" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z110" s="2"/>
+      <c r="AA110" s="2"/>
+      <c r="AB110" s="2"/>
+      <c r="AC110" s="2"/>
+      <c r="AD110" s="2"/>
+      <c r="AE110" s="2"/>
+    </row>
+    <row r="111" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z111" s="2"/>
+      <c r="AA111" s="2"/>
+      <c r="AB111" s="2"/>
+      <c r="AC111" s="2"/>
+      <c r="AD111" s="2"/>
+      <c r="AE111" s="2"/>
+    </row>
+    <row r="112" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z112" s="2"/>
+      <c r="AA112" s="2"/>
+      <c r="AB112" s="2"/>
+      <c r="AC112" s="2"/>
+      <c r="AD112" s="2"/>
+      <c r="AE112" s="2"/>
+    </row>
+    <row r="113" spans="26:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z113" s="2"/>
+      <c r="AA113" s="2"/>
+      <c r="AB113" s="2"/>
+      <c r="AC113" s="2"/>
+      <c r="AD113" s="2"/>
+      <c r="AE113" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:E13">
@@ -3532,7 +3637,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S84:X89">
+  <conditionalFormatting sqref="S94:X99">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3544,7 +3649,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S93:X98">
+  <conditionalFormatting sqref="S103:X108">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3604,7 +3709,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z98:AE103">
+  <conditionalFormatting sqref="Z108:AE113">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3641,14 +3746,2756 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:AY113"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="P77" workbookViewId="0">
+      <selection activeCell="X86" sqref="X86"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="51" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:51" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AT2" s="6"/>
+      <c r="AU2" s="6"/>
+      <c r="AV2" s="6"/>
+      <c r="AW2" s="6"/>
+      <c r="AX2" s="6"/>
+      <c r="AY2" s="6"/>
+    </row>
+    <row r="4" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4.9186949530000003E-2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.57265660750000003</v>
+      </c>
+      <c r="E8" s="2">
+        <f>SUM(D8:D13)</f>
+        <v>0.95081304958629997</v>
+      </c>
+    </row>
+    <row r="9" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.30851659809999998</v>
+      </c>
+      <c r="E9" s="2">
+        <f>SUM(D9:D13)</f>
+        <v>0.37815644208629995</v>
+      </c>
+    </row>
+    <row r="10" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2">
+        <v>6.2518520820000006E-2</v>
+      </c>
+      <c r="E10" s="2">
+        <f>SUM(D10:D13)</f>
+        <v>6.9639843986299993E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="D11" s="2">
+        <v>6.7587590079999996E-3</v>
+      </c>
+      <c r="E11" s="2">
+        <f>SUM(D11:D13)</f>
+        <v>7.1213231662999995E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3.5572415829999998E-4</v>
+      </c>
+      <c r="E12" s="2">
+        <f>SUM(D12:D13)</f>
+        <v>3.6256415829999996E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13" s="2">
+        <v>6.8399999999999997E-6</v>
+      </c>
+      <c r="E13" s="2">
+        <f>SUM(D13)</f>
+        <v>6.8399999999999997E-6</v>
+      </c>
+    </row>
+    <row r="14" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="3:51" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AT17" s="6"/>
+      <c r="AU17" s="6"/>
+      <c r="AV17" s="6"/>
+      <c r="AW17" s="6"/>
+      <c r="AX17" s="6"/>
+      <c r="AY17" s="6"/>
+    </row>
+    <row r="19" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="AT19"/>
+      <c r="AY19"/>
+    </row>
+    <row r="20" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+      <c r="S20" t="s">
+        <v>23</v>
+      </c>
+      <c r="AT20"/>
+      <c r="AY20"/>
+    </row>
+    <row r="21" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="S21" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT21"/>
+      <c r="AY21"/>
+    </row>
+    <row r="22" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>0.110767768470584</v>
+      </c>
+      <c r="G22">
+        <v>0.131280318187359</v>
+      </c>
+      <c r="H22">
+        <v>0.15472323214938699</v>
+      </c>
+      <c r="I22">
+        <v>0.18139965148548901</v>
+      </c>
+      <c r="J22">
+        <v>0.29355534998458199</v>
+      </c>
+      <c r="K22">
+        <v>0.44033302497687299</v>
+      </c>
+      <c r="L22">
+        <v>0.61609620721554104</v>
+      </c>
+      <c r="M22">
+        <v>0.80851063829787195</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>1</v>
+      </c>
+      <c r="U22">
+        <v>2</v>
+      </c>
+      <c r="V22">
+        <v>3</v>
+      </c>
+      <c r="W22">
+        <v>4</v>
+      </c>
+      <c r="X22">
+        <v>5</v>
+      </c>
+      <c r="Y22">
+        <v>6</v>
+      </c>
+      <c r="Z22">
+        <v>7</v>
+      </c>
+      <c r="AA22">
+        <v>8</v>
+      </c>
+      <c r="AT22"/>
+      <c r="AY22"/>
+    </row>
+    <row r="23" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>0.26666314631807297</v>
+      </c>
+      <c r="G23">
+        <v>0.28131496754434099</v>
+      </c>
+      <c r="H23">
+        <v>0.29344061269711502</v>
+      </c>
+      <c r="I23">
+        <v>0.30233275247581498</v>
+      </c>
+      <c r="J23">
+        <v>0.33024976873265399</v>
+      </c>
+      <c r="K23">
+        <v>0.31082331174838101</v>
+      </c>
+      <c r="L23">
+        <v>0.23959296947271</v>
+      </c>
+      <c r="M23">
+        <v>0.12765957446808501</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>5</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23" s="2">
+        <v>0.15645464858454</v>
+      </c>
+      <c r="T23" s="2">
+        <v>0.18542773165575199</v>
+      </c>
+      <c r="U23" s="2">
+        <v>0.21853982659427901</v>
+      </c>
+      <c r="V23" s="2">
+        <v>0.25621910704156797</v>
+      </c>
+      <c r="W23" s="2">
+        <v>0.38570618264322099</v>
+      </c>
+      <c r="X23" s="2">
+        <v>0.53911205073995705</v>
+      </c>
+      <c r="Y23" s="2">
+        <v>0.70401691331923799</v>
+      </c>
+      <c r="Z23" s="2">
+        <v>0.86363636363636298</v>
+      </c>
+      <c r="AA23" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD23" s="1">
+        <v>0.110767768470584</v>
+      </c>
+      <c r="AE23" s="1">
+        <v>0.131280318187359</v>
+      </c>
+      <c r="AF23" s="1">
+        <v>0.15472323214938699</v>
+      </c>
+      <c r="AG23" s="1">
+        <v>0.18139965148548901</v>
+      </c>
+      <c r="AH23" s="1">
+        <v>0.29355534998458199</v>
+      </c>
+      <c r="AI23" s="1">
+        <v>0.44033302497687299</v>
+      </c>
+      <c r="AJ23" s="1">
+        <v>0.61609620721554104</v>
+      </c>
+      <c r="AK23" s="1">
+        <v>0.80851063829787195</v>
+      </c>
+      <c r="AL23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AT23"/>
+      <c r="AY23"/>
+    </row>
+    <row r="24" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>0.22856841112977699</v>
+      </c>
+      <c r="G24">
+        <v>0.21341135468881001</v>
+      </c>
+      <c r="H24">
+        <v>0.19562707513141001</v>
+      </c>
+      <c r="I24">
+        <v>0.17554804982466701</v>
+      </c>
+      <c r="J24">
+        <v>0.120090824993692</v>
+      </c>
+      <c r="K24">
+        <v>6.21646623496762E-2</v>
+      </c>
+      <c r="L24">
+        <v>1.94264569842738E-2</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>1</v>
+      </c>
+      <c r="S24" s="2">
+        <v>0.37665007992574601</v>
+      </c>
+      <c r="T24" s="2">
+        <v>0.39734513926232501</v>
+      </c>
+      <c r="U24" s="2">
+        <v>0.414472084920184</v>
+      </c>
+      <c r="V24" s="2">
+        <v>0.42703184506928099</v>
+      </c>
+      <c r="W24" s="2">
+        <v>0.43391945547362398</v>
+      </c>
+      <c r="X24" s="2">
+        <v>0.38054968287526397</v>
+      </c>
+      <c r="Y24" s="2">
+        <v>0.27378435517970401</v>
+      </c>
+      <c r="Z24" s="2">
+        <v>0.13636363636363599</v>
+      </c>
+      <c r="AA24" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="1">
+        <v>0.26666314631807297</v>
+      </c>
+      <c r="AE24" s="1">
+        <v>0.28131496754434099</v>
+      </c>
+      <c r="AF24" s="1">
+        <v>0.29344061269711502</v>
+      </c>
+      <c r="AG24" s="1">
+        <v>0.30233275247581498</v>
+      </c>
+      <c r="AH24" s="1">
+        <v>0.33024976873265399</v>
+      </c>
+      <c r="AI24" s="1">
+        <v>0.31082331174838101</v>
+      </c>
+      <c r="AJ24" s="1">
+        <v>0.23959296947271</v>
+      </c>
+      <c r="AK24" s="1">
+        <v>0.12765957446808501</v>
+      </c>
+      <c r="AL24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT24"/>
+      <c r="AY24"/>
+    </row>
+    <row r="25" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>8.6698362842329402E-2</v>
+      </c>
+      <c r="G25">
+        <v>7.1137118229603599E-2</v>
+      </c>
+      <c r="H25">
+        <v>5.6794957296215802E-2</v>
+      </c>
+      <c r="I25">
+        <v>4.3887012456166698E-2</v>
+      </c>
+      <c r="J25">
+        <v>1.6483054410898999E-2</v>
+      </c>
+      <c r="K25">
+        <v>3.4535923527597898E-3</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>2</v>
+      </c>
+      <c r="S25" s="2">
+        <v>0.32284292565063899</v>
+      </c>
+      <c r="T25" s="2">
+        <v>0.301434243578316</v>
+      </c>
+      <c r="U25" s="2">
+        <v>0.27631472328012302</v>
+      </c>
+      <c r="V25" s="2">
+        <v>0.24795397455635601</v>
+      </c>
+      <c r="W25" s="2">
+        <v>0.15778889289949899</v>
+      </c>
+      <c r="X25" s="2">
+        <v>7.61099365750528E-2</v>
+      </c>
+      <c r="Y25" s="2">
+        <v>2.2198731501057001E-2</v>
+      </c>
+      <c r="Z25" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="1">
+        <v>0.22856841112977699</v>
+      </c>
+      <c r="AE25" s="1">
+        <v>0.21341135468881001</v>
+      </c>
+      <c r="AF25" s="1">
+        <v>0.19562707513141001</v>
+      </c>
+      <c r="AG25" s="1">
+        <v>0.17554804982466701</v>
+      </c>
+      <c r="AH25" s="1">
+        <v>0.120090824993692</v>
+      </c>
+      <c r="AI25" s="1">
+        <v>6.21646623496762E-2</v>
+      </c>
+      <c r="AJ25" s="1">
+        <v>1.94264569842738E-2</v>
+      </c>
+      <c r="AK25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT25"/>
+      <c r="AY25"/>
+    </row>
+    <row r="26" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>1.44497271403882E-2</v>
+      </c>
+      <c r="G26">
+        <v>1.03263558720392E-2</v>
+      </c>
+      <c r="H26">
+        <v>7.09936966202697E-3</v>
+      </c>
+      <c r="I26">
+        <v>4.6546831392904097E-3</v>
+      </c>
+      <c r="J26">
+        <v>7.0641661760995696E-4</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>3</v>
+      </c>
+      <c r="S26" s="2">
+        <v>0.12245766145369</v>
+      </c>
+      <c r="T26" s="2">
+        <v>0.100478081192772</v>
+      </c>
+      <c r="U26" s="2">
+        <v>8.0220403532938897E-2</v>
+      </c>
+      <c r="V26" s="2">
+        <v>6.1988493639089197E-2</v>
+      </c>
+      <c r="W26" s="2">
+        <v>2.16572990254215E-2</v>
+      </c>
+      <c r="X26" s="2">
+        <v>4.2283298097251501E-3</v>
+      </c>
+      <c r="Y26" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="1">
+        <v>8.6698362842329402E-2</v>
+      </c>
+      <c r="AE26" s="1">
+        <v>7.1137118229603599E-2</v>
+      </c>
+      <c r="AF26" s="1">
+        <v>5.6794957296215802E-2</v>
+      </c>
+      <c r="AG26" s="1">
+        <v>4.3887012456166698E-2</v>
+      </c>
+      <c r="AH26" s="1">
+        <v>1.6483054410898999E-2</v>
+      </c>
+      <c r="AI26" s="1">
+        <v>3.4535923527597898E-3</v>
+      </c>
+      <c r="AJ26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT26"/>
+      <c r="AY26"/>
+    </row>
+    <row r="27" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>8.3901641460318798E-4</v>
+      </c>
+      <c r="G27">
+        <v>5.16317793601962E-4</v>
+      </c>
+      <c r="H27">
+        <v>3.0118537960114401E-4</v>
+      </c>
+      <c r="I27">
+        <v>1.64282934327897E-4</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>4</v>
+      </c>
+      <c r="S27" s="2">
+        <v>2.04096102422818E-2</v>
+      </c>
+      <c r="T27" s="2">
+        <v>1.4585527915079799E-2</v>
+      </c>
+      <c r="U27" s="2">
+        <v>1.00275504416173E-2</v>
+      </c>
+      <c r="V27" s="2">
+        <v>6.5745372041458201E-3</v>
+      </c>
+      <c r="W27" s="2">
+        <v>9.2816995823235095E-4</v>
+      </c>
+      <c r="X27" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="1">
+        <v>1.44497271403882E-2</v>
+      </c>
+      <c r="AE27" s="1">
+        <v>1.03263558720392E-2</v>
+      </c>
+      <c r="AF27" s="1">
+        <v>7.09936966202697E-3</v>
+      </c>
+      <c r="AG27" s="1">
+        <v>4.6546831392904097E-3</v>
+      </c>
+      <c r="AH27" s="1">
+        <v>7.0641661760995696E-4</v>
+      </c>
+      <c r="AI27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT27"/>
+      <c r="AY27"/>
+    </row>
+    <row r="28" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="R28">
+        <v>5</v>
+      </c>
+      <c r="S28" s="2">
+        <v>1.18507414310023E-3</v>
+      </c>
+      <c r="T28" s="2">
+        <v>7.2927639575398997E-4</v>
+      </c>
+      <c r="U28" s="2">
+        <v>4.2541123085649402E-4</v>
+      </c>
+      <c r="V28" s="2">
+        <v>2.3204248955808701E-4</v>
+      </c>
+      <c r="W28" s="2">
+        <v>0</v>
+      </c>
+      <c r="X28" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD28" s="1">
+        <v>8.3901641460318798E-4</v>
+      </c>
+      <c r="AE28" s="1">
+        <v>5.16317793601962E-4</v>
+      </c>
+      <c r="AF28" s="1">
+        <v>3.0118537960114401E-4</v>
+      </c>
+      <c r="AG28" s="1">
+        <v>1.64282934327897E-4</v>
+      </c>
+      <c r="AH28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY28"/>
+    </row>
+    <row r="29" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="AY29"/>
+    </row>
+    <row r="30" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="AU30"/>
+    </row>
+    <row r="31" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="S31" t="s">
+        <v>26</v>
+      </c>
+      <c r="AU31"/>
+    </row>
+    <row r="32" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="AU32"/>
+    </row>
+    <row r="33" spans="3:47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="3:47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="3:47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S36">
+        <v>0</v>
+      </c>
+      <c r="T36">
+        <v>0</v>
+      </c>
+      <c r="U36">
+        <v>4.9186949530000003E-2</v>
+      </c>
+      <c r="V36">
+        <v>0.57265660750000003</v>
+      </c>
+      <c r="W36">
+        <v>0.30851659809999998</v>
+      </c>
+      <c r="X36">
+        <v>6.2518520820000006E-2</v>
+      </c>
+      <c r="Y36">
+        <v>6.7587590079999996E-3</v>
+      </c>
+      <c r="Z36">
+        <v>3.5572415829999998E-4</v>
+      </c>
+      <c r="AA36" s="3">
+        <v>6.8399999999999997E-6</v>
+      </c>
+      <c r="AT36" s="7"/>
+      <c r="AU36" s="7"/>
+    </row>
+    <row r="37" spans="3:47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S37" t="s">
+        <v>22</v>
+      </c>
+      <c r="AT37" s="7"/>
+      <c r="AU37" s="7"/>
+    </row>
+    <row r="38" spans="3:47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R38" t="s">
+        <v>4</v>
+      </c>
+      <c r="S38">
+        <v>0</v>
+      </c>
+      <c r="T38">
+        <v>1</v>
+      </c>
+      <c r="U38">
+        <v>2</v>
+      </c>
+      <c r="V38">
+        <v>3</v>
+      </c>
+      <c r="W38">
+        <v>4</v>
+      </c>
+      <c r="X38">
+        <v>5</v>
+      </c>
+      <c r="Y38">
+        <v>6</v>
+      </c>
+      <c r="Z38">
+        <v>7</v>
+      </c>
+      <c r="AA38">
+        <v>8</v>
+      </c>
+      <c r="AT38" s="7"/>
+      <c r="AU38" s="7"/>
+    </row>
+    <row r="39" spans="3:47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q39" t="s">
+        <v>5</v>
+      </c>
+      <c r="R39">
+        <v>0</v>
+      </c>
+      <c r="S39" s="2">
+        <f>SUM(S23:S28)</f>
+        <v>0.999999999999997</v>
+      </c>
+      <c r="T39" s="2">
+        <f t="shared" ref="T39:AA39" si="0">SUM(T23:T28)</f>
+        <v>0.99999999999999889</v>
+      </c>
+      <c r="U39" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999878</v>
+      </c>
+      <c r="V39" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999811</v>
+      </c>
+      <c r="W39" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999778</v>
+      </c>
+      <c r="X39" s="2">
+        <f t="shared" si="0"/>
+        <v>0.999999999999999</v>
+      </c>
+      <c r="Y39" s="2">
+        <f t="shared" si="0"/>
+        <v>0.999999999999999</v>
+      </c>
+      <c r="Z39" s="2">
+        <f t="shared" si="0"/>
+        <v>0.999999999999999</v>
+      </c>
+      <c r="AA39" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AT39" s="7"/>
+      <c r="AU39" s="7"/>
+    </row>
+    <row r="40" spans="3:47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R40">
+        <v>1</v>
+      </c>
+      <c r="S40" s="2">
+        <f t="shared" ref="S40:AA44" si="1">SUM(S24:S29)</f>
+        <v>0.84354535141545706</v>
+      </c>
+      <c r="T40" s="2">
+        <f t="shared" si="1"/>
+        <v>0.8145722683442469</v>
+      </c>
+      <c r="U40" s="2">
+        <f t="shared" si="1"/>
+        <v>0.78146017340571972</v>
+      </c>
+      <c r="V40" s="2">
+        <f t="shared" si="1"/>
+        <v>0.74378089295843008</v>
+      </c>
+      <c r="W40" s="2">
+        <f t="shared" si="1"/>
+        <v>0.61429381735677668</v>
+      </c>
+      <c r="X40" s="2">
+        <f t="shared" si="1"/>
+        <v>0.4608879492600419</v>
+      </c>
+      <c r="Y40" s="2">
+        <f t="shared" si="1"/>
+        <v>0.29598308668076101</v>
+      </c>
+      <c r="Z40" s="2">
+        <f t="shared" si="1"/>
+        <v>0.13636363636363599</v>
+      </c>
+      <c r="AA40" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AT40" s="7"/>
+      <c r="AU40" s="7"/>
+    </row>
+    <row r="41" spans="3:47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R41">
+        <v>2</v>
+      </c>
+      <c r="S41" s="2">
+        <f t="shared" si="1"/>
+        <v>0.46689527148971099</v>
+      </c>
+      <c r="T41" s="2">
+        <f t="shared" si="1"/>
+        <v>0.41722712908192178</v>
+      </c>
+      <c r="U41" s="2">
+        <f t="shared" si="1"/>
+        <v>0.36698808848553571</v>
+      </c>
+      <c r="V41" s="2">
+        <f t="shared" si="1"/>
+        <v>0.31674904788914909</v>
+      </c>
+      <c r="W41" s="2">
+        <f t="shared" si="1"/>
+        <v>0.18037436188315284</v>
+      </c>
+      <c r="X41" s="2">
+        <f t="shared" si="1"/>
+        <v>8.0338266384777951E-2</v>
+      </c>
+      <c r="Y41" s="2">
+        <f t="shared" si="1"/>
+        <v>2.2198731501057001E-2</v>
+      </c>
+      <c r="Z41" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA41" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AT41" s="7"/>
+      <c r="AU41" s="7"/>
+    </row>
+    <row r="42" spans="3:47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R42">
+        <v>3</v>
+      </c>
+      <c r="S42" s="2">
+        <f t="shared" si="1"/>
+        <v>0.14405234583907203</v>
+      </c>
+      <c r="T42" s="2">
+        <f t="shared" si="1"/>
+        <v>0.11579288550360579</v>
+      </c>
+      <c r="U42" s="2">
+        <f t="shared" si="1"/>
+        <v>9.0673365205412679E-2</v>
+      </c>
+      <c r="V42" s="2">
+        <f t="shared" si="1"/>
+        <v>6.8795073332793111E-2</v>
+      </c>
+      <c r="W42" s="2">
+        <f t="shared" si="1"/>
+        <v>2.258546898365385E-2</v>
+      </c>
+      <c r="X42" s="2">
+        <f t="shared" si="1"/>
+        <v>4.2283298097251501E-3</v>
+      </c>
+      <c r="Y42" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Z42" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA42" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AT42" s="7"/>
+      <c r="AU42" s="7"/>
+    </row>
+    <row r="43" spans="3:47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R43">
+        <v>4</v>
+      </c>
+      <c r="S43" s="2">
+        <f t="shared" si="1"/>
+        <v>2.1594684385382031E-2</v>
+      </c>
+      <c r="T43" s="2">
+        <f t="shared" si="1"/>
+        <v>1.5314804310833789E-2</v>
+      </c>
+      <c r="U43" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0452961672473794E-2</v>
+      </c>
+      <c r="V43" s="2">
+        <f t="shared" si="1"/>
+        <v>6.8065796937039069E-3</v>
+      </c>
+      <c r="W43" s="2">
+        <f t="shared" si="1"/>
+        <v>9.2816995823235095E-4</v>
+      </c>
+      <c r="X43" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y43" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Z43" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA43" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AT43" s="7"/>
+      <c r="AU43" s="7"/>
+    </row>
+    <row r="44" spans="3:47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R44">
+        <v>5</v>
+      </c>
+      <c r="S44" s="2">
+        <f t="shared" si="1"/>
+        <v>1.18507414310023E-3</v>
+      </c>
+      <c r="T44" s="2">
+        <f t="shared" si="1"/>
+        <v>7.2927639575398997E-4</v>
+      </c>
+      <c r="U44" s="2">
+        <f t="shared" si="1"/>
+        <v>4.2541123085649402E-4</v>
+      </c>
+      <c r="V44" s="2">
+        <f t="shared" si="1"/>
+        <v>2.3204248955808701E-4</v>
+      </c>
+      <c r="W44" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X44" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y44" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Z44" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA44" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AT44" s="7"/>
+      <c r="AU44" s="7"/>
+    </row>
+    <row r="46" spans="3:47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S46" t="s">
+        <v>24</v>
+      </c>
+      <c r="AT46" s="7"/>
+      <c r="AU46" s="7"/>
+    </row>
+    <row r="47" spans="3:47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="R47" t="s">
+        <v>4</v>
+      </c>
+      <c r="S47">
+        <v>0</v>
+      </c>
+      <c r="T47">
+        <v>1</v>
+      </c>
+      <c r="U47">
+        <v>2</v>
+      </c>
+      <c r="V47">
+        <v>3</v>
+      </c>
+      <c r="W47">
+        <v>4</v>
+      </c>
+      <c r="X47">
+        <v>5</v>
+      </c>
+      <c r="Y47">
+        <v>6</v>
+      </c>
+      <c r="Z47">
+        <v>7</v>
+      </c>
+      <c r="AA47">
+        <v>8</v>
+      </c>
+      <c r="AT47" s="7"/>
+      <c r="AU47" s="7"/>
+    </row>
+    <row r="48" spans="3:47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q48" t="s">
+        <v>5</v>
+      </c>
+      <c r="R48">
+        <v>0</v>
+      </c>
+      <c r="S48" s="2">
+        <f t="shared" ref="S48:S53" si="2">S39*$S$36</f>
+        <v>0</v>
+      </c>
+      <c r="T48" s="2">
+        <f t="shared" ref="T48:T53" si="3">T39*$T$36</f>
+        <v>0</v>
+      </c>
+      <c r="U48" s="2">
+        <f t="shared" ref="U48:U53" si="4">U39*$U$36</f>
+        <v>4.918694952999994E-2</v>
+      </c>
+      <c r="V48" s="2">
+        <f t="shared" ref="V48:V53" si="5">V39*$V$36</f>
+        <v>0.57265660749999892</v>
+      </c>
+      <c r="W48" s="2">
+        <f t="shared" ref="W48:W53" si="6">W39*W$36</f>
+        <v>0.30851659809999932</v>
+      </c>
+      <c r="X48" s="2">
+        <f t="shared" ref="X48:X53" si="7">X39*$X$36</f>
+        <v>6.2518520819999937E-2</v>
+      </c>
+      <c r="Y48" s="2">
+        <f t="shared" ref="Y48:Y53" si="8">Y39*$Y$36</f>
+        <v>6.7587590079999926E-3</v>
+      </c>
+      <c r="Z48" s="2">
+        <f t="shared" ref="Z48:Z53" si="9">Z39*$Z$36</f>
+        <v>3.557241582999996E-4</v>
+      </c>
+      <c r="AA48" s="2">
+        <f t="shared" ref="AA48:AA53" si="10">AA39*$AA$36</f>
+        <v>6.8399999999999997E-6</v>
+      </c>
+      <c r="AT48" s="7"/>
+      <c r="AU48" s="7"/>
+    </row>
+    <row r="49" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N49" s="3"/>
+      <c r="R49">
+        <v>1</v>
+      </c>
+      <c r="S49" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T49" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U49" s="2">
+        <f t="shared" si="4"/>
+        <v>3.8437642109012189E-2</v>
+      </c>
+      <c r="V49" s="2">
+        <f t="shared" si="5"/>
+        <v>0.42593104288489525</v>
+      </c>
+      <c r="W49" s="8">
+        <f t="shared" si="6"/>
+        <v>0.18951983876477546</v>
+      </c>
+      <c r="X49" s="2">
+        <f t="shared" si="7"/>
+        <v>2.8814032851501036E-2</v>
+      </c>
+      <c r="Y49" s="2">
+        <f t="shared" si="8"/>
+        <v>2.000478353319238E-3</v>
+      </c>
+      <c r="Z49" s="2">
+        <f t="shared" si="9"/>
+        <v>4.8507839768181685E-5</v>
+      </c>
+      <c r="AA49" s="2">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R50">
+        <v>2</v>
+      </c>
+      <c r="S50" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T50" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U50" s="2">
+        <f t="shared" si="4"/>
+        <v>1.8051024586449221E-2</v>
+      </c>
+      <c r="V50" s="8">
+        <f t="shared" si="5"/>
+        <v>0.18138843519305517</v>
+      </c>
+      <c r="W50" s="2">
+        <f t="shared" si="6"/>
+        <v>5.5648484512648623E-2</v>
+      </c>
+      <c r="X50" s="2">
+        <f t="shared" si="7"/>
+        <v>5.0226295796194469E-3</v>
+      </c>
+      <c r="Y50" s="2">
+        <f t="shared" si="8"/>
+        <v>1.5003587649894235E-4</v>
+      </c>
+      <c r="Z50" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA50" s="2">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R51">
+        <v>3</v>
+      </c>
+      <c r="S51" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T51" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U51" s="8">
+        <f t="shared" si="4"/>
+        <v>4.4599462380738916E-3</v>
+      </c>
+      <c r="V51" s="2">
+        <f t="shared" si="5"/>
+        <v>3.9395953307471025E-2</v>
+      </c>
+      <c r="W51" s="2">
+        <f t="shared" si="6"/>
+        <v>6.9679920573299499E-3</v>
+      </c>
+      <c r="X51" s="2">
+        <f t="shared" si="7"/>
+        <v>2.6434892524312845E-4</v>
+      </c>
+      <c r="Y51" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Z51" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA51" s="2">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R52">
+        <v>4</v>
+      </c>
+      <c r="S52" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T52" s="8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U52" s="2">
+        <f t="shared" si="4"/>
+        <v>5.1414929822299294E-4</v>
+      </c>
+      <c r="V52" s="2">
+        <f t="shared" si="5"/>
+        <v>3.8978328360748686E-3</v>
+      </c>
+      <c r="W52" s="2">
+        <f t="shared" si="6"/>
+        <v>2.8635583797246401E-4</v>
+      </c>
+      <c r="X52" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y52" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Z52" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA52" s="2">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R53">
+        <v>5</v>
+      </c>
+      <c r="S53" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T53" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U53" s="2">
+        <f t="shared" si="4"/>
+        <v>2.0924680741633553E-5</v>
+      </c>
+      <c r="V53" s="2">
+        <f t="shared" si="5"/>
+        <v>1.328806648661883E-4</v>
+      </c>
+      <c r="W53" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X53" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y53" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Z53" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA53" s="2">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AC53" s="2">
+        <f>SUM(S53,T52,U51,V50,W49,)</f>
+        <v>0.37536822019590455</v>
+      </c>
+    </row>
+    <row r="54" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S54" s="8"/>
+      <c r="T54" s="2"/>
+      <c r="U54" s="2"/>
+      <c r="V54" s="2"/>
+      <c r="W54" s="2"/>
+      <c r="X54" s="2"/>
+      <c r="Y54" s="2"/>
+      <c r="Z54" s="2"/>
+      <c r="AA54" s="2"/>
+      <c r="AC54" s="2"/>
+    </row>
+    <row r="55" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S55" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T55" s="2"/>
+      <c r="U55" s="2"/>
+      <c r="V55" s="2"/>
+      <c r="W55" s="2"/>
+      <c r="X55" s="2"/>
+      <c r="Y55" s="2"/>
+      <c r="Z55" s="2"/>
+      <c r="AA55" s="2"/>
+      <c r="AC55" s="2"/>
+    </row>
+    <row r="56" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R56" t="s">
+        <v>4</v>
+      </c>
+      <c r="S56">
+        <v>0</v>
+      </c>
+      <c r="T56">
+        <v>1</v>
+      </c>
+      <c r="U56">
+        <v>2</v>
+      </c>
+      <c r="V56">
+        <v>3</v>
+      </c>
+      <c r="W56">
+        <v>4</v>
+      </c>
+      <c r="X56">
+        <v>5</v>
+      </c>
+      <c r="Y56">
+        <v>6</v>
+      </c>
+      <c r="Z56">
+        <v>7</v>
+      </c>
+      <c r="AA56">
+        <v>8</v>
+      </c>
+      <c r="AC56" s="2"/>
+    </row>
+    <row r="57" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q57" t="s">
+        <v>5</v>
+      </c>
+      <c r="R57">
+        <v>0</v>
+      </c>
+      <c r="S57" s="2">
+        <f>S23*$S$36</f>
+        <v>0</v>
+      </c>
+      <c r="T57" s="2">
+        <f>T23*$T$36</f>
+        <v>0</v>
+      </c>
+      <c r="U57" s="2">
+        <f>U23*$U$36</f>
+        <v>1.0749307420987755E-2</v>
+      </c>
+      <c r="V57" s="2">
+        <f>V23*$V$36</f>
+        <v>0.14672556461510369</v>
+      </c>
+      <c r="W57" s="2">
+        <f>W23*$W$36</f>
+        <v>0.1189967593352238</v>
+      </c>
+      <c r="X57" s="2">
+        <f>X23*$X$36</f>
+        <v>3.3704487968498904E-2</v>
+      </c>
+      <c r="Y57" s="2">
+        <f>Y23*$Y$36</f>
+        <v>4.7582806546807551E-3</v>
+      </c>
+      <c r="Z57" s="2">
+        <f>Z23*$Z$36</f>
+        <v>3.0721631853181791E-4</v>
+      </c>
+      <c r="AA57" s="2">
+        <f>AA23*$AA$36</f>
+        <v>6.8399999999999997E-6</v>
+      </c>
+      <c r="AC57" s="2"/>
+    </row>
+    <row r="58" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R58">
+        <v>1</v>
+      </c>
+      <c r="S58" s="2">
+        <f t="shared" ref="S58:S62" si="11">S24*$S$36</f>
+        <v>0</v>
+      </c>
+      <c r="T58" s="2">
+        <f t="shared" ref="T58:T62" si="12">T24*$T$36</f>
+        <v>0</v>
+      </c>
+      <c r="U58" s="2">
+        <f>U24*$U$36</f>
+        <v>2.0386617522562964E-2</v>
+      </c>
+      <c r="V58" s="2">
+        <f t="shared" ref="V58:V62" si="13">V24*$V$36</f>
+        <v>0.24454260769184005</v>
+      </c>
+      <c r="W58" s="2">
+        <f t="shared" ref="W58:W62" si="14">W24*$W$36</f>
+        <v>0.1338713542521269</v>
+      </c>
+      <c r="X58" s="2">
+        <f t="shared" ref="X58:X62" si="15">X24*$X$36</f>
+        <v>2.3791403271881589E-2</v>
+      </c>
+      <c r="Y58" s="2">
+        <f t="shared" ref="Y58:Y62" si="16">Y24*$Y$36</f>
+        <v>1.8504424768202958E-3</v>
+      </c>
+      <c r="Z58" s="2">
+        <f t="shared" ref="Z58:Z62" si="17">Z24*$Z$36</f>
+        <v>4.8507839768181685E-5</v>
+      </c>
+      <c r="AA58" s="2">
+        <f t="shared" ref="AA58:AA62" si="18">AA24*$AA$36</f>
+        <v>0</v>
+      </c>
+      <c r="AC58" s="2"/>
+    </row>
+    <row r="59" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R59">
+        <v>2</v>
+      </c>
+      <c r="S59" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="T59" s="2">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="U59" s="2">
+        <f t="shared" ref="U58:U62" si="19">U25*$U$36</f>
+        <v>1.3591078348375328E-2</v>
+      </c>
+      <c r="V59" s="2">
+        <f t="shared" si="13"/>
+        <v>0.14199248188558417</v>
+      </c>
+      <c r="W59" s="2">
+        <f t="shared" si="14"/>
+        <v>4.868049245531867E-2</v>
+      </c>
+      <c r="X59" s="2">
+        <f t="shared" si="15"/>
+        <v>4.758280654376318E-3</v>
+      </c>
+      <c r="Y59" s="2">
+        <f t="shared" si="16"/>
+        <v>1.5003587649894235E-4</v>
+      </c>
+      <c r="Z59" s="2">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AA59" s="2">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AC59" s="2"/>
+    </row>
+    <row r="60" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R60">
+        <v>3</v>
+      </c>
+      <c r="S60" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="T60" s="2">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="U60" s="2">
+        <f t="shared" si="19"/>
+        <v>3.945796939850899E-3</v>
+      </c>
+      <c r="V60" s="2">
+        <f t="shared" si="13"/>
+        <v>3.5498120471396152E-2</v>
+      </c>
+      <c r="W60" s="2">
+        <f t="shared" si="14"/>
+        <v>6.6816362193574865E-3</v>
+      </c>
+      <c r="X60" s="2">
+        <f t="shared" si="15"/>
+        <v>2.6434892524312845E-4</v>
+      </c>
+      <c r="Y60" s="2">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="Z60" s="2">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AA60" s="2">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AC60" s="2"/>
+    </row>
+    <row r="61" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R61">
+        <v>4</v>
+      </c>
+      <c r="S61" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="T61" s="2">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="U61" s="2">
+        <f t="shared" si="19"/>
+        <v>4.9322461748135934E-4</v>
+      </c>
+      <c r="V61" s="2">
+        <f t="shared" si="13"/>
+        <v>3.7649521712086803E-3</v>
+      </c>
+      <c r="W61" s="2">
+        <f t="shared" si="14"/>
+        <v>2.8635583797246401E-4</v>
+      </c>
+      <c r="X61" s="2">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="Y61" s="2">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="Z61" s="2">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AA61" s="2">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AC61" s="2"/>
+    </row>
+    <row r="62" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R62">
+        <v>5</v>
+      </c>
+      <c r="S62" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="T62" s="2">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="U62" s="2">
+        <f t="shared" si="19"/>
+        <v>2.0924680741633553E-5</v>
+      </c>
+      <c r="V62" s="2">
+        <f t="shared" si="13"/>
+        <v>1.328806648661883E-4</v>
+      </c>
+      <c r="W62" s="2">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="X62" s="2">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="Y62" s="2">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="Z62" s="2">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="AA62" s="2">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AC62" s="2"/>
+    </row>
+    <row r="63" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AC63" s="2"/>
+    </row>
+    <row r="64" spans="14:29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AC64" s="2"/>
+    </row>
+    <row r="65" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="AA65" s="3"/>
+    </row>
+    <row r="67" spans="3:51" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C67" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AT67" s="6"/>
+      <c r="AU67" s="6"/>
+      <c r="AV67" s="6"/>
+      <c r="AW67" s="6"/>
+      <c r="AX67" s="6"/>
+      <c r="AY67" s="6"/>
+    </row>
+    <row r="70" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="R70" t="s">
+        <v>21</v>
+      </c>
+      <c r="S70" t="s">
+        <v>15</v>
+      </c>
+      <c r="T70" t="s">
+        <v>16</v>
+      </c>
+      <c r="U70" t="s">
+        <v>17</v>
+      </c>
+      <c r="V70" t="s">
+        <v>18</v>
+      </c>
+      <c r="W70" t="s">
+        <v>19</v>
+      </c>
+      <c r="X70" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="Q71" t="s">
+        <v>14</v>
+      </c>
+      <c r="R71">
+        <v>0</v>
+      </c>
+      <c r="S71" s="2">
+        <v>0.17069701280227501</v>
+      </c>
+      <c r="T71" s="2">
+        <v>0.20625889046941601</v>
+      </c>
+      <c r="U71" s="2">
+        <v>0.34429368639894897</v>
+      </c>
+      <c r="V71" s="2">
+        <v>0.20625889046941601</v>
+      </c>
+      <c r="W71" s="2">
+        <v>0.33318743845059601</v>
+      </c>
+      <c r="X71" s="2">
+        <v>0.33318743845059601</v>
+      </c>
+      <c r="Z71" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="72" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="R72">
+        <v>1</v>
+      </c>
+      <c r="S72" s="2">
+        <v>0.39118065433854898</v>
+      </c>
+      <c r="T72" s="2">
+        <v>0.41251778093883301</v>
+      </c>
+      <c r="U72" s="2">
+        <v>0.44266331108436302</v>
+      </c>
+      <c r="V72" s="2">
+        <v>0.41251778093883301</v>
+      </c>
+      <c r="W72" s="2">
+        <v>0.44424991793412799</v>
+      </c>
+      <c r="X72" s="2">
+        <v>0.44424991793412799</v>
+      </c>
+    </row>
+    <row r="73" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="R73">
+        <v>2</v>
+      </c>
+      <c r="S73" s="2">
+        <v>0.31294452347083901</v>
+      </c>
+      <c r="T73" s="2">
+        <v>0.28558923295765398</v>
+      </c>
+      <c r="U73" s="2">
+        <v>0.18317102527628801</v>
+      </c>
+      <c r="V73" s="2">
+        <v>0.28558923295765398</v>
+      </c>
+      <c r="W73" s="2">
+        <v>0.19039282197176899</v>
+      </c>
+      <c r="X73" s="2">
+        <v>0.19039282197176899</v>
+      </c>
+    </row>
+    <row r="74" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="R74">
+        <v>3</v>
+      </c>
+      <c r="S74" s="2">
+        <v>0.10832695043221301</v>
+      </c>
+      <c r="T74" s="2">
+        <v>8.4619031987453006E-2</v>
+      </c>
+      <c r="U74" s="2">
+        <v>2.8493270598533699E-2</v>
+      </c>
+      <c r="V74" s="2">
+        <v>8.4619031987453006E-2</v>
+      </c>
+      <c r="W74" s="2">
+        <v>3.0637925374767401E-2</v>
+      </c>
+      <c r="X74" s="2">
+        <v>3.0637925374767401E-2</v>
+      </c>
+      <c r="AC74" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="R75">
+        <v>4</v>
+      </c>
+      <c r="S75" s="2">
+        <v>1.60484371010686E-2</v>
+      </c>
+      <c r="T75" s="2">
+        <v>1.05773789984316E-2</v>
+      </c>
+      <c r="U75" s="2">
+        <v>1.37870664186453E-3</v>
+      </c>
+      <c r="V75" s="2">
+        <v>1.05773789984316E-2</v>
+      </c>
+      <c r="W75" s="2">
+        <v>1.5318962687383699E-3</v>
+      </c>
+      <c r="X75" s="2">
+        <v>1.5318962687383699E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="3:51" x14ac:dyDescent="0.25">
+      <c r="R76">
+        <v>5</v>
+      </c>
+      <c r="S76" s="2">
+        <v>8.0242185505343397E-4</v>
+      </c>
+      <c r="T76" s="2">
+        <v>4.37684648210964E-4</v>
+      </c>
+      <c r="U76" s="2">
+        <v>0</v>
+      </c>
+      <c r="V76" s="2">
+        <v>4.37684648210964E-4</v>
+      </c>
+      <c r="W76" s="2">
+        <v>0</v>
+      </c>
+      <c r="X76" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="9:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R84" t="s">
+        <v>21</v>
+      </c>
+      <c r="S84" t="s">
+        <v>15</v>
+      </c>
+      <c r="T84" t="s">
+        <v>16</v>
+      </c>
+      <c r="U84" t="s">
+        <v>17</v>
+      </c>
+      <c r="V84" t="s">
+        <v>18</v>
+      </c>
+      <c r="W84" t="s">
+        <v>19</v>
+      </c>
+      <c r="X84" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="85" spans="9:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q85" t="s">
+        <v>14</v>
+      </c>
+      <c r="R85">
+        <v>0</v>
+      </c>
+      <c r="S85" s="2">
+        <f>$S$92*S71</f>
+        <v>1.8348746664559365E-3</v>
+      </c>
+      <c r="T85" s="2">
+        <f>$T$92*T71</f>
+        <v>3.0263452161009893E-2</v>
+      </c>
+      <c r="U85" s="2">
+        <f>$U$92*U71</f>
+        <v>4.0969832941052747E-2</v>
+      </c>
+      <c r="V85" s="2">
+        <f>$V$92*V71</f>
+        <v>4.2049211106281919E-3</v>
+      </c>
+      <c r="W85" s="2">
+        <f>$W$92*W71</f>
+        <v>8.1478525048873207E-2</v>
+      </c>
+      <c r="X85" s="2">
+        <f>$X$92*X71</f>
+        <v>4.5283765806765327E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="9:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R86">
+        <v>1</v>
+      </c>
+      <c r="S86" s="2">
+        <f t="shared" ref="S86:S90" si="20">$S$92*S72</f>
+        <v>4.2049211106282101E-3</v>
+      </c>
+      <c r="T86" s="2">
+        <f t="shared" ref="T86:T90" si="21">$T$92*T72</f>
+        <v>6.0526904322019931E-2</v>
+      </c>
+      <c r="U86" s="8">
+        <f t="shared" ref="U86:U90" si="22">$U$92*U72</f>
+        <v>5.2675499495639252E-2</v>
+      </c>
+      <c r="V86" s="2">
+        <f t="shared" ref="V86:V90" si="23">$V$92*V72</f>
+        <v>8.4098422212564028E-3</v>
+      </c>
+      <c r="W86" s="8">
+        <f t="shared" ref="W86:W90" si="24">$W$92*W72</f>
+        <v>0.1086380333984976</v>
+      </c>
+      <c r="X86" s="8">
+        <f t="shared" ref="X86:X90" si="25">$X$92*X72</f>
+        <v>6.0378354409020433E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="9:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R87">
+        <v>2</v>
+      </c>
+      <c r="S87" s="2">
+        <f t="shared" si="20"/>
+        <v>3.3639368885025663E-3</v>
+      </c>
+      <c r="T87" s="8">
+        <f t="shared" si="21"/>
+        <v>4.1903241453706164E-2</v>
+      </c>
+      <c r="U87" s="2">
+        <f t="shared" si="22"/>
+        <v>2.1796758411988641E-2</v>
+      </c>
+      <c r="V87" s="8">
+        <f t="shared" si="23"/>
+        <v>5.8221984608698247E-3</v>
+      </c>
+      <c r="W87" s="2">
+        <f t="shared" si="24"/>
+        <v>4.6559157170784647E-2</v>
+      </c>
+      <c r="X87" s="2">
+        <f t="shared" si="25"/>
+        <v>2.587643760386588E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="9:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R88">
+        <v>3</v>
+      </c>
+      <c r="S88" s="8">
+        <f t="shared" si="20"/>
+        <v>1.1644396921739598E-3</v>
+      </c>
+      <c r="T88" s="2">
+        <f t="shared" si="21"/>
+        <v>1.2415775245542562E-2</v>
+      </c>
+      <c r="U88" s="2">
+        <f t="shared" si="22"/>
+        <v>3.390606864087123E-3</v>
+      </c>
+      <c r="V88" s="2">
+        <f t="shared" si="23"/>
+        <v>1.7250958402577254E-3</v>
+      </c>
+      <c r="W88" s="2">
+        <f t="shared" si="24"/>
+        <v>7.4922781654136157E-3</v>
+      </c>
+      <c r="X88" s="2">
+        <f t="shared" si="25"/>
+        <v>4.1640244420014028E-4</v>
+      </c>
+    </row>
+    <row r="89" spans="9:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R89">
+        <v>4</v>
+      </c>
+      <c r="S89" s="2">
+        <f t="shared" si="20"/>
+        <v>1.7250958402577191E-4</v>
+      </c>
+      <c r="T89" s="2">
+        <f t="shared" si="21"/>
+        <v>1.5519719056928164E-3</v>
+      </c>
+      <c r="U89" s="2">
+        <f t="shared" si="22"/>
+        <v>1.6406162245582808E-4</v>
+      </c>
+      <c r="V89" s="2">
+        <f t="shared" si="23"/>
+        <v>2.1563698003221514E-4</v>
+      </c>
+      <c r="W89" s="2">
+        <f t="shared" si="24"/>
+        <v>3.7461390827068077E-4</v>
+      </c>
+      <c r="X89" s="2">
+        <f t="shared" si="25"/>
+        <v>2.0820122210007011E-5</v>
+      </c>
+    </row>
+    <row r="90" spans="9:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R90">
+        <v>5</v>
+      </c>
+      <c r="S90" s="2">
+        <f t="shared" si="20"/>
+        <v>8.6254792012886384E-6</v>
+      </c>
+      <c r="T90" s="2">
+        <f t="shared" si="21"/>
+        <v>6.4219527132116727E-5</v>
+      </c>
+      <c r="U90" s="2">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="V90" s="2">
+        <f t="shared" si="23"/>
+        <v>8.9229095185744448E-6</v>
+      </c>
+      <c r="W90" s="2">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="X90" s="2">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="9:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S92" s="2">
+        <f>U57</f>
+        <v>1.0749307420987755E-2</v>
+      </c>
+      <c r="T92" s="2">
+        <f>V57</f>
+        <v>0.14672556461510369</v>
+      </c>
+      <c r="U92" s="2">
+        <f>W57</f>
+        <v>0.1189967593352238</v>
+      </c>
+      <c r="V92" s="2">
+        <f>U58</f>
+        <v>2.0386617522562964E-2</v>
+      </c>
+      <c r="W92" s="2">
+        <f>V58</f>
+        <v>0.24454260769184005</v>
+      </c>
+      <c r="X92" s="2">
+        <f>U59</f>
+        <v>1.3591078348375328E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="9:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I93" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q93" t="s">
+        <v>14</v>
+      </c>
+      <c r="R93" t="s">
+        <v>21</v>
+      </c>
+      <c r="S93" t="s">
+        <v>15</v>
+      </c>
+      <c r="T93" t="s">
+        <v>16</v>
+      </c>
+      <c r="U93" t="s">
+        <v>17</v>
+      </c>
+      <c r="V93" t="s">
+        <v>18</v>
+      </c>
+      <c r="W93" t="s">
+        <v>19</v>
+      </c>
+      <c r="X93" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="94" spans="9:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I94" s="9">
+        <f>T73*T92</f>
+        <v>4.1903241453706164E-2</v>
+      </c>
+      <c r="R94">
+        <v>0</v>
+      </c>
+      <c r="S94" s="2">
+        <f>SUM(S71:S76)</f>
+        <v>0.999999999999998</v>
+      </c>
+      <c r="T94" s="2">
+        <f>SUM(T71:T76)</f>
+        <v>0.99999999999999845</v>
+      </c>
+      <c r="U94" s="2">
+        <f t="shared" ref="U94:X98" si="26">SUM(U71:U76)</f>
+        <v>0.99999999999999822</v>
+      </c>
+      <c r="V94" s="2">
+        <f t="shared" si="26"/>
+        <v>0.99999999999999845</v>
+      </c>
+      <c r="W94" s="2">
+        <f t="shared" si="26"/>
+        <v>0.99999999999999878</v>
+      </c>
+      <c r="X94" s="2">
+        <f t="shared" si="26"/>
+        <v>0.99999999999999878</v>
+      </c>
+      <c r="Z94" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="95" spans="9:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R95">
+        <v>1</v>
+      </c>
+      <c r="S95" s="10">
+        <f t="shared" ref="S95:T98" si="27">SUM(S72:S77)</f>
+        <v>0.829302987197723</v>
+      </c>
+      <c r="T95" s="2">
+        <f t="shared" si="27"/>
+        <v>0.79374110953058252</v>
+      </c>
+      <c r="U95" s="2">
+        <f t="shared" si="26"/>
+        <v>0.65570631360104925</v>
+      </c>
+      <c r="V95" s="2">
+        <f t="shared" si="26"/>
+        <v>0.79374110953058252</v>
+      </c>
+      <c r="W95" s="2">
+        <f t="shared" si="26"/>
+        <v>0.66681256154940272</v>
+      </c>
+      <c r="X95" s="2">
+        <f t="shared" si="26"/>
+        <v>0.66681256154940272</v>
+      </c>
+    </row>
+    <row r="96" spans="9:26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R96">
+        <v>2</v>
+      </c>
+      <c r="S96" s="2">
+        <f t="shared" si="27"/>
+        <v>0.43812233285917407</v>
+      </c>
+      <c r="T96" s="2">
+        <f t="shared" si="27"/>
+        <v>0.38122332859174957</v>
+      </c>
+      <c r="U96" s="2">
+        <f t="shared" si="26"/>
+        <v>0.21304300251668626</v>
+      </c>
+      <c r="V96" s="2">
+        <f>SUM(V73:V78)</f>
+        <v>0.38122332859174957</v>
+      </c>
+      <c r="W96" s="2">
+        <f t="shared" si="26"/>
+        <v>0.22256264361527475</v>
+      </c>
+      <c r="X96" s="2">
+        <f t="shared" si="26"/>
+        <v>0.22256264361527475</v>
+      </c>
+    </row>
+    <row r="97" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R97">
+        <v>3</v>
+      </c>
+      <c r="S97" s="2">
+        <f t="shared" si="27"/>
+        <v>0.12517780938833503</v>
+      </c>
+      <c r="T97" s="2">
+        <f t="shared" si="27"/>
+        <v>9.563409563409557E-2</v>
+      </c>
+      <c r="U97" s="2">
+        <f t="shared" si="26"/>
+        <v>2.987197724039823E-2</v>
+      </c>
+      <c r="V97" s="2">
+        <f t="shared" si="26"/>
+        <v>9.563409563409557E-2</v>
+      </c>
+      <c r="W97" s="2">
+        <f t="shared" si="26"/>
+        <v>3.2169821643505771E-2</v>
+      </c>
+      <c r="X97" s="2">
+        <f t="shared" si="26"/>
+        <v>3.2169821643505771E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R98">
+        <v>4</v>
+      </c>
+      <c r="S98" s="2">
+        <f t="shared" si="27"/>
+        <v>1.6850858956122036E-2</v>
+      </c>
+      <c r="T98" s="2">
+        <f t="shared" si="27"/>
+        <v>1.1015063646642564E-2</v>
+      </c>
+      <c r="U98" s="2">
+        <f t="shared" si="26"/>
+        <v>1.37870664186453E-3</v>
+      </c>
+      <c r="V98" s="2">
+        <f t="shared" si="26"/>
+        <v>1.1015063646642564E-2</v>
+      </c>
+      <c r="W98" s="2">
+        <f t="shared" si="26"/>
+        <v>1.5318962687383699E-3</v>
+      </c>
+      <c r="X98" s="2">
+        <f t="shared" si="26"/>
+        <v>1.5318962687383699E-3</v>
+      </c>
+    </row>
+    <row r="99" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R99">
+        <v>5</v>
+      </c>
+      <c r="S99" s="2">
+        <f t="shared" ref="S99:X99" si="28">SUM(S76:S91)</f>
+        <v>1.1551729276041168E-2</v>
+      </c>
+      <c r="T99" s="2">
+        <f t="shared" si="28"/>
+        <v>0.14716324926331442</v>
+      </c>
+      <c r="U99" s="2">
+        <f t="shared" si="28"/>
+        <v>0.11899675933522359</v>
+      </c>
+      <c r="V99" s="2">
+        <f t="shared" si="28"/>
+        <v>2.0824302170773898E-2</v>
+      </c>
+      <c r="W99" s="2">
+        <f>SUM(W76:W91)</f>
+        <v>0.24454260769183975</v>
+      </c>
+      <c r="X99" s="2">
+        <f t="shared" si="28"/>
+        <v>1.3591078348375311E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q102" t="s">
+        <v>14</v>
+      </c>
+      <c r="R102" t="s">
+        <v>21</v>
+      </c>
+      <c r="S102" t="s">
+        <v>15</v>
+      </c>
+      <c r="T102" t="s">
+        <v>16</v>
+      </c>
+      <c r="U102" t="s">
+        <v>17</v>
+      </c>
+      <c r="V102" t="s">
+        <v>18</v>
+      </c>
+      <c r="W102" t="s">
+        <v>19</v>
+      </c>
+      <c r="X102" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="103" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R103">
+        <v>0</v>
+      </c>
+      <c r="S103" s="2">
+        <f>$S$92*S94</f>
+        <v>1.0749307420987734E-2</v>
+      </c>
+      <c r="T103" s="2">
+        <f>$T$92*T94</f>
+        <v>0.14672556461510347</v>
+      </c>
+      <c r="U103" s="2">
+        <f>$U$92*U94</f>
+        <v>0.11899675933522359</v>
+      </c>
+      <c r="V103" s="2">
+        <f>$V$92*V94</f>
+        <v>2.0386617522562933E-2</v>
+      </c>
+      <c r="W103" s="2">
+        <f>$W$92*W94</f>
+        <v>0.24454260769183975</v>
+      </c>
+      <c r="X103" s="2">
+        <f>$X$92*X94</f>
+        <v>1.3591078348375311E-2</v>
+      </c>
+      <c r="Z103" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="104" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R104">
+        <v>1</v>
+      </c>
+      <c r="S104" s="2">
+        <f t="shared" ref="S104:S108" si="29">$S$92*S95</f>
+        <v>8.9144327545317963E-3</v>
+      </c>
+      <c r="T104" s="2">
+        <f t="shared" ref="T104:T108" si="30">$T$92*T95</f>
+        <v>0.11646211245409359</v>
+      </c>
+      <c r="U104" s="8">
+        <f t="shared" ref="U104:U108" si="31">$U$92*U95</f>
+        <v>7.8026926394170845E-2</v>
+      </c>
+      <c r="V104" s="2">
+        <f t="shared" ref="V104:V108" si="32">$V$92*V95</f>
+        <v>1.6181696411934742E-2</v>
+      </c>
+      <c r="W104" s="8">
+        <f t="shared" ref="W104:W108" si="33">$W$92*W95</f>
+        <v>0.16306408264296654</v>
+      </c>
+      <c r="X104" s="8">
+        <f t="shared" ref="X104:X108" si="34">$X$92*X95</f>
+        <v>9.0627017676987772E-3</v>
+      </c>
+    </row>
+    <row r="105" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R105">
+        <v>2</v>
+      </c>
+      <c r="S105" s="2">
+        <f t="shared" si="29"/>
+        <v>4.7095116439035871E-3</v>
+      </c>
+      <c r="T105" s="8">
+        <f t="shared" si="30"/>
+        <v>5.5935208132073658E-2</v>
+      </c>
+      <c r="U105" s="2">
+        <f t="shared" si="31"/>
+        <v>2.5351426898531593E-2</v>
+      </c>
+      <c r="V105" s="8">
+        <f t="shared" si="32"/>
+        <v>7.7718541906783402E-3</v>
+      </c>
+      <c r="W105" s="2">
+        <f t="shared" si="33"/>
+        <v>5.4426049244468942E-2</v>
+      </c>
+      <c r="X105" s="2">
+        <f t="shared" si="34"/>
+        <v>3.0248663267967353E-3</v>
+      </c>
+    </row>
+    <row r="106" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R106">
+        <v>3</v>
+      </c>
+      <c r="S106" s="8">
+        <f t="shared" si="29"/>
+        <v>1.3455747554010204E-3</v>
+      </c>
+      <c r="T106" s="2">
+        <f t="shared" si="30"/>
+        <v>1.4031966678367496E-2</v>
+      </c>
+      <c r="U106" s="2">
+        <f t="shared" si="31"/>
+        <v>3.5546684865429509E-3</v>
+      </c>
+      <c r="V106" s="2">
+        <f t="shared" si="32"/>
+        <v>1.9496557298085151E-3</v>
+      </c>
+      <c r="W106" s="2">
+        <f t="shared" si="33"/>
+        <v>7.8668920736842968E-3</v>
+      </c>
+      <c r="X106" s="2">
+        <f t="shared" si="34"/>
+        <v>4.3722256641014727E-4</v>
+      </c>
+    </row>
+    <row r="107" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R107">
+        <v>4</v>
+      </c>
+      <c r="S107" s="2">
+        <f t="shared" si="29"/>
+        <v>1.8113506322706057E-4</v>
+      </c>
+      <c r="T107" s="2">
+        <f t="shared" si="30"/>
+        <v>1.6161914328249333E-3</v>
+      </c>
+      <c r="U107" s="2">
+        <f t="shared" si="31"/>
+        <v>1.6406162245582808E-4</v>
+      </c>
+      <c r="V107" s="2">
+        <f t="shared" si="32"/>
+        <v>2.245598895507896E-4</v>
+      </c>
+      <c r="W107" s="2">
+        <f t="shared" si="33"/>
+        <v>3.7461390827068077E-4</v>
+      </c>
+      <c r="X107" s="2">
+        <f t="shared" si="34"/>
+        <v>2.0820122210007011E-5</v>
+      </c>
+    </row>
+    <row r="108" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R108">
+        <v>5</v>
+      </c>
+      <c r="S108" s="2">
+        <f t="shared" si="29"/>
+        <v>1.2417308923219083E-4</v>
+      </c>
+      <c r="T108" s="2">
+        <f t="shared" si="30"/>
+        <v>2.1592610838753051E-2</v>
+      </c>
+      <c r="U108" s="2">
+        <f t="shared" si="31"/>
+        <v>1.4160228732285148E-2</v>
+      </c>
+      <c r="V108" s="2">
+        <f t="shared" si="32"/>
+        <v>4.245370835298451E-4</v>
+      </c>
+      <c r="W108" s="2">
+        <f t="shared" si="33"/>
+        <v>5.9801086976725114E-2</v>
+      </c>
+      <c r="X108" s="2">
+        <f t="shared" si="34"/>
+        <v>1.8471741067167639E-4</v>
+      </c>
+      <c r="Z108" s="2">
+        <f>SUM(S106,T105,U104,V105,W104,X104)</f>
+        <v>0.31520634788298924</v>
+      </c>
+      <c r="AA108" s="2"/>
+      <c r="AB108" s="2"/>
+      <c r="AC108" s="2"/>
+      <c r="AD108" s="2"/>
+      <c r="AE108" s="2"/>
+    </row>
+    <row r="109" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z109" s="2"/>
+      <c r="AA109" s="2"/>
+      <c r="AB109" s="2"/>
+      <c r="AC109" s="2"/>
+      <c r="AD109" s="2"/>
+      <c r="AE109" s="2"/>
+    </row>
+    <row r="110" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z110" s="2"/>
+      <c r="AA110" s="2"/>
+      <c r="AB110" s="2"/>
+      <c r="AC110" s="2"/>
+      <c r="AD110" s="2"/>
+      <c r="AE110" s="2"/>
+    </row>
+    <row r="111" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z111" s="2"/>
+      <c r="AA111" s="2"/>
+      <c r="AB111" s="2"/>
+      <c r="AC111" s="2"/>
+      <c r="AD111" s="2"/>
+      <c r="AE111" s="2"/>
+    </row>
+    <row r="112" spans="17:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z112" s="2"/>
+      <c r="AA112" s="2"/>
+      <c r="AB112" s="2"/>
+      <c r="AC112" s="2"/>
+      <c r="AD112" s="2"/>
+      <c r="AE112" s="2"/>
+    </row>
+    <row r="113" spans="26:31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z113" s="2"/>
+      <c r="AA113" s="2"/>
+      <c r="AB113" s="2"/>
+      <c r="AC113" s="2"/>
+      <c r="AD113" s="2"/>
+      <c r="AE113" s="2"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D5:E13">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S71:X76">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S94:X99">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S103:X108">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S23:AA28">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S39:AA44">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S48:AA55">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S57:AA62">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z108:AE113">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC53:AC64">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD23:AL28">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S85:X90">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20:J58"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>